<commit_message>
test ieee14 base v0: works
</commit_message>
<xml_diff>
--- a/bshe/Test_ieee14_vsg/ieee14_vsg.xlsx
+++ b/bshe/Test_ieee14_vsg/ieee14_vsg.xlsx
@@ -16,7 +16,7 @@
     <sheet name="ACE" sheetId="11" r:id="rId11"/>
     <sheet name="ACEc" sheetId="12" r:id="rId12"/>
     <sheet name="COI" sheetId="13" r:id="rId13"/>
-    <sheet name="REGCV2" sheetId="14" r:id="rId14"/>
+    <sheet name="REGCV1" sheetId="14" r:id="rId14"/>
     <sheet name="GENROU" sheetId="15" r:id="rId15"/>
     <sheet name="TGOV1N" sheetId="16" r:id="rId16"/>
     <sheet name="EXST1" sheetId="17" r:id="rId17"/>
@@ -658,7 +658,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -707,27 +707,39 @@
         <v>D</v>
       </c>
       <c r="O1" t="str">
+        <v>Kpid</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Kiid</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>Kpiq</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Kiiq</v>
+      </c>
+      <c r="S1" t="str">
         <v>Kpvd</v>
       </c>
-      <c r="P1" t="str">
+      <c r="T1" t="str">
         <v>Kivd</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="U1" t="str">
         <v>Kpvq</v>
       </c>
-      <c r="R1" t="str">
+      <c r="V1" t="str">
         <v>Kivq</v>
       </c>
-      <c r="S1" t="str">
+      <c r="W1" t="str">
         <v>ra</v>
       </c>
-      <c r="T1" t="str">
+      <c r="X1" t="str">
         <v>xs</v>
       </c>
-      <c r="U1" t="str">
+      <c r="Y1" t="str">
         <v>gammap</v>
       </c>
-      <c r="V1" t="str">
+      <c r="Z1" t="str">
         <v>gammaq</v>
       </c>
     </row>
@@ -772,33 +784,45 @@
         <v>0.5</v>
       </c>
       <c r="O2" t="str">
-        <v>0.1</v>
+        <v>100</v>
       </c>
       <c r="P2" t="str">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="Q2" t="str">
-        <v>0.1</v>
+        <v>100</v>
       </c>
       <c r="R2" t="str">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="S2" t="str">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="T2" t="str">
+        <v>500</v>
+      </c>
+      <c r="U2" t="str">
+        <v>1000</v>
+      </c>
+      <c r="V2" t="str">
+        <v>500</v>
+      </c>
+      <c r="W2" t="str">
+        <v>0</v>
+      </c>
+      <c r="X2" t="str">
         <v>0.15</v>
       </c>
-      <c r="U2" t="str">
-        <v>1</v>
-      </c>
-      <c r="V2" t="str">
+      <c r="Y2" t="str">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="str">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:V2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Z2"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2336,7 +2360,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2410,9 +2434,32 @@
         <v>1.1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>2</v>
+      </c>
+      <c r="B4" t="str">
+        <v>3</v>
+      </c>
+      <c r="C4" t="str">
+        <v>1</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Toggler_2</v>
+      </c>
+      <c r="E4" t="str">
+        <v>SynGen</v>
+      </c>
+      <c r="F4" t="str">
+        <v>GENROU_2</v>
+      </c>
+      <c r="G4" t="str">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add test  vsg v0: work
</commit_message>
<xml_diff>
--- a/bshe/Test_ieee14_vsg/ieee14_vsg.xlsx
+++ b/bshe/Test_ieee14_vsg/ieee14_vsg.xlsx
@@ -707,16 +707,16 @@
         <v>D</v>
       </c>
       <c r="O1" t="str">
-        <v>Kpid</v>
+        <v>KpId</v>
       </c>
       <c r="P1" t="str">
-        <v>Kiid</v>
+        <v>KiId</v>
       </c>
       <c r="Q1" t="str">
-        <v>Kpiq</v>
+        <v>KpIq</v>
       </c>
       <c r="R1" t="str">
-        <v>Kiiq</v>
+        <v>KiIq</v>
       </c>
       <c r="S1" t="str">
         <v>Kpvd</v>

</xml_diff>